<commit_message>
Issue #2 - Last input play mode implementation.
</commit_message>
<xml_diff>
--- a/IHE8001チェック5A2.xlsx
+++ b/IHE8001チェック5A2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\VoiceNavi\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\VoiceNavi\voice_navi_test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0040254-BF07-4418-92CD-F987EC2A4267}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDA29C87-E2CE-45F0-A72F-9DA3E479E501}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0FCDEBC5-A1B8-419C-8E9C-F2839559D4D0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0FCDEBC5-A1B8-419C-8E9C-F2839559D4D0}"/>
   </bookViews>
   <sheets>
     <sheet name="IHE8001 チェック" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="78">
   <si>
     <t>IHE8001 チェック事項</t>
     <rPh sb="12" eb="14">
@@ -241,34 +241,6 @@
   </si>
   <si>
     <t>-</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">001優先順位再 </t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">010順次記憶再生 </t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>011記憶エンドレス(複数交互)</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">100記憶エンドレス(優先順位) </t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">101入力切替 </t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">110バイナリ制御 1(正論理） </t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>111なし</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -479,6 +451,27 @@
   </si>
   <si>
     <t>JumperMS2,1</t>
+  </si>
+  <si>
+    <t>010優先順位再生</t>
+  </si>
+  <si>
+    <t>001後入力切替再生</t>
+  </si>
+  <si>
+    <t>011入力中再生</t>
+  </si>
+  <si>
+    <t>100バイナリ制御127(負論理）</t>
+  </si>
+  <si>
+    <t>101空き</t>
+  </si>
+  <si>
+    <t xml:space="preserve">110バイナリ制御 250(負論理） </t>
+  </si>
+  <si>
+    <t xml:space="preserve">111バイナリ制御 250(正論理） </t>
   </si>
 </sst>
 </file>
@@ -957,8 +950,8 @@
   </sheetPr>
   <dimension ref="A1:H48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -983,10 +976,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="D3" s="9" t="s">
         <v>2</v>
@@ -1024,7 +1017,7 @@
         <v>11</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="H4" s="1"/>
     </row>
@@ -1044,7 +1037,7 @@
         <v>12</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="H5" s="1"/>
     </row>
@@ -1064,7 +1057,7 @@
         <v>13</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="H6" s="1"/>
     </row>
@@ -1122,7 +1115,7 @@
         <v>16</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="H9" s="1"/>
     </row>
@@ -1164,7 +1157,7 @@
       </c>
       <c r="F11" s="5"/>
       <c r="G11" s="1" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="H11" s="1"/>
     </row>
@@ -1184,7 +1177,7 @@
       </c>
       <c r="F12" s="5"/>
       <c r="G12" s="1" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="H12" s="1"/>
     </row>
@@ -1204,7 +1197,7 @@
       </c>
       <c r="F13" s="5"/>
       <c r="G13" s="1" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="H13" s="1"/>
     </row>
@@ -1224,7 +1217,7 @@
       </c>
       <c r="F14" s="5"/>
       <c r="G14" s="1" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="H14" s="1"/>
     </row>
@@ -1244,7 +1237,7 @@
       </c>
       <c r="F15" s="5"/>
       <c r="G15" s="1" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="H15" s="1"/>
     </row>
@@ -1264,7 +1257,7 @@
       </c>
       <c r="F16" s="5"/>
       <c r="G16" s="1" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="H16" s="1"/>
     </row>
@@ -1273,10 +1266,10 @@
         <v>13</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>35</v>
@@ -1288,7 +1281,7 @@
         <v>30</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="H17" s="1"/>
     </row>
@@ -1375,10 +1368,10 @@
         <v>20</v>
       </c>
       <c r="B23" s="15" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>35</v>
@@ -1387,11 +1380,13 @@
         <v>24</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="G23" s="1"/>
+        <v>59</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>69</v>
+      </c>
       <c r="H23" s="12" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -1400,7 +1395,7 @@
       </c>
       <c r="B24" s="15"/>
       <c r="C24" s="7" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>35</v>
@@ -1418,7 +1413,7 @@
       </c>
       <c r="B25" s="15"/>
       <c r="C25" s="7" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>35</v>
@@ -1436,7 +1431,7 @@
       </c>
       <c r="B26" s="15"/>
       <c r="C26" s="7" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>35</v>
@@ -1454,7 +1449,7 @@
       </c>
       <c r="B27" s="15"/>
       <c r="C27" s="7" t="s">
-        <v>41</v>
+        <v>72</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>35</v>
@@ -1463,7 +1458,9 @@
         <v>24</v>
       </c>
       <c r="F27" s="5"/>
-      <c r="G27" s="1"/>
+      <c r="G27" s="1" t="s">
+        <v>69</v>
+      </c>
       <c r="H27" s="14"/>
     </row>
     <row r="28" spans="1:8">
@@ -1472,7 +1469,7 @@
       </c>
       <c r="B28" s="15"/>
       <c r="C28" s="7" t="s">
-        <v>42</v>
+        <v>71</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>35</v>
@@ -1490,7 +1487,7 @@
       </c>
       <c r="B29" s="15"/>
       <c r="C29" s="7" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>35</v>
@@ -1508,7 +1505,7 @@
       </c>
       <c r="B30" s="15"/>
       <c r="C30" s="7" t="s">
-        <v>44</v>
+        <v>74</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>35</v>
@@ -1516,7 +1513,9 @@
       <c r="E30" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F30" s="5"/>
+      <c r="F30" s="5" t="s">
+        <v>62</v>
+      </c>
       <c r="G30" s="1"/>
       <c r="H30" s="14"/>
     </row>
@@ -1526,7 +1525,7 @@
       </c>
       <c r="B31" s="15"/>
       <c r="C31" s="7" t="s">
-        <v>45</v>
+        <v>75</v>
       </c>
       <c r="D31" s="3" t="s">
         <v>35</v>
@@ -1535,7 +1534,9 @@
         <v>24</v>
       </c>
       <c r="F31" s="5"/>
-      <c r="G31" s="1"/>
+      <c r="G31" s="1" t="s">
+        <v>69</v>
+      </c>
       <c r="H31" s="13"/>
     </row>
     <row r="32" spans="1:8">
@@ -1544,7 +1545,7 @@
       </c>
       <c r="B32" s="15"/>
       <c r="C32" s="7" t="s">
-        <v>46</v>
+        <v>76</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>35</v>
@@ -1553,11 +1554,11 @@
         <v>24</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="G32" s="1"/>
       <c r="H32" s="1" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
     </row>
     <row r="33" spans="1:8">
@@ -1566,7 +1567,7 @@
       </c>
       <c r="B33" s="16"/>
       <c r="C33" s="7" t="s">
-        <v>47</v>
+        <v>77</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>35</v>
@@ -1574,7 +1575,9 @@
       <c r="E33" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F33" s="5"/>
+      <c r="F33" s="5" t="s">
+        <v>62</v>
+      </c>
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
     </row>
@@ -1583,19 +1586,19 @@
         <v>31</v>
       </c>
       <c r="B34" s="11" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="D34" s="3" t="s">
         <v>35</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
@@ -1644,7 +1647,7 @@
       </c>
       <c r="B37" s="14"/>
       <c r="C37" s="1" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="D37" s="3" t="s">
         <v>39</v>
@@ -1653,9 +1656,11 @@
         <v>24</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="G37" s="1"/>
+        <v>46</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>69</v>
+      </c>
       <c r="H37" s="1"/>
     </row>
     <row r="38" spans="1:8">
@@ -1691,9 +1696,11 @@
         <v>24</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="G39" s="1"/>
+        <v>51</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>69</v>
+      </c>
       <c r="H39" s="1"/>
     </row>
     <row r="40" spans="1:8">
@@ -1711,9 +1718,11 @@
         <v>24</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="G40" s="1"/>
+        <v>50</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>69</v>
+      </c>
       <c r="H40" s="1"/>
     </row>
     <row r="41" spans="1:8">
@@ -1721,10 +1730,10 @@
         <v>38</v>
       </c>
       <c r="B41" s="12" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="D41" s="11" t="s">
         <v>35</v>
@@ -1733,10 +1742,10 @@
         <v>24</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="H41" s="1"/>
     </row>
@@ -1746,16 +1755,16 @@
       </c>
       <c r="B42" s="13"/>
       <c r="C42" s="1" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="D42" s="11" t="s">
         <v>35</v>
       </c>
       <c r="E42" s="11" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="G42" s="1"/>
       <c r="H42" s="1"/>
@@ -1765,7 +1774,7 @@
         <v>40</v>
       </c>
       <c r="B43" s="10" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>31</v>
@@ -1785,7 +1794,7 @@
         <v>41</v>
       </c>
       <c r="B44" s="10" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>32</v>
@@ -1794,7 +1803,7 @@
         <v>35</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="F44" s="5"/>
       <c r="G44" s="1"/>
@@ -1805,7 +1814,7 @@
         <v>42</v>
       </c>
       <c r="B45" s="10" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>33</v>
@@ -1814,7 +1823,7 @@
         <v>35</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="F45" s="5"/>
       <c r="G45" s="1"/>

</xml_diff>

<commit_message>
Issue #2 - Priority play mode implementation.
</commit_message>
<xml_diff>
--- a/IHE8001チェック5A2.xlsx
+++ b/IHE8001チェック5A2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\VoiceNavi\voice_navi_test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDA29C87-E2CE-45F0-A72F-9DA3E479E501}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1214642-317B-45C3-82E9-91A2854F94FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0FCDEBC5-A1B8-419C-8E9C-F2839559D4D0}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="78">
   <si>
     <t>IHE8001 チェック事項</t>
     <rPh sb="12" eb="14">
@@ -951,7 +951,7 @@
   <dimension ref="A1:H48"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G38" sqref="G38"/>
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -1478,7 +1478,9 @@
         <v>24</v>
       </c>
       <c r="F28" s="5"/>
-      <c r="G28" s="1"/>
+      <c r="G28" s="1" t="s">
+        <v>69</v>
+      </c>
       <c r="H28" s="14"/>
     </row>
     <row r="29" spans="1:8">

</xml_diff>

<commit_message>
Issue #2 - Input play mode implementation.
</commit_message>
<xml_diff>
--- a/IHE8001チェック5A2.xlsx
+++ b/IHE8001チェック5A2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\VoiceNavi\voice_navi_test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1214642-317B-45C3-82E9-91A2854F94FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C26D7F06-7182-4B17-90CC-649A34549997}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0FCDEBC5-A1B8-419C-8E9C-F2839559D4D0}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="78">
   <si>
     <t>IHE8001 チェック事項</t>
     <rPh sb="12" eb="14">
@@ -951,7 +951,7 @@
   <dimension ref="A1:H48"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -1498,7 +1498,9 @@
         <v>24</v>
       </c>
       <c r="F29" s="5"/>
-      <c r="G29" s="1"/>
+      <c r="G29" s="1" t="s">
+        <v>69</v>
+      </c>
       <c r="H29" s="14"/>
     </row>
     <row r="30" spans="1:8">

</xml_diff>

<commit_message>
Issue #2 - All binary play modes implementation.
</commit_message>
<xml_diff>
--- a/IHE8001チェック5A2.xlsx
+++ b/IHE8001チェック5A2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\VoiceNavi\voice_navi_test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C26D7F06-7182-4B17-90CC-649A34549997}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ACBF5EF-8F55-449A-B943-696E818D9115}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0FCDEBC5-A1B8-419C-8E9C-F2839559D4D0}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="78">
   <si>
     <t>IHE8001 チェック事項</t>
     <rPh sb="12" eb="14">
@@ -951,7 +951,7 @@
   <dimension ref="A1:H48"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -1520,7 +1520,9 @@
       <c r="F30" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="G30" s="1"/>
+      <c r="G30" s="1" t="s">
+        <v>69</v>
+      </c>
       <c r="H30" s="14"/>
     </row>
     <row r="31" spans="1:8">
@@ -1560,7 +1562,9 @@
       <c r="F32" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="G32" s="1"/>
+      <c r="G32" s="1" t="s">
+        <v>69</v>
+      </c>
       <c r="H32" s="1" t="s">
         <v>61</v>
       </c>
@@ -1582,7 +1586,9 @@
       <c r="F33" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="G33" s="1"/>
+      <c r="G33" s="1" t="s">
+        <v>69</v>
+      </c>
       <c r="H33" s="1"/>
     </row>
     <row r="34" spans="1:8">

</xml_diff>

<commit_message>
Flash - always wire on new page. Don't write on same page twice.
</commit_message>
<xml_diff>
--- a/IHE8001チェック5A2.xlsx
+++ b/IHE8001チェック5A2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\VoiceNavi\voice_navi_test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ACBF5EF-8F55-449A-B943-696E818D9115}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD0D09A2-1524-41AA-9B66-DBF1707F2578}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0FCDEBC5-A1B8-419C-8E9C-F2839559D4D0}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="79">
   <si>
     <t>IHE8001 チェック事項</t>
     <rPh sb="12" eb="14">
@@ -472,6 +472,9 @@
   </si>
   <si>
     <t xml:space="preserve">111バイナリ制御 250(正論理） </t>
+  </si>
+  <si>
+    <t>no</t>
   </si>
 </sst>
 </file>
@@ -950,8 +953,8 @@
   </sheetPr>
   <dimension ref="A1:H48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -1076,7 +1079,9 @@
       <c r="F7" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G7" s="1"/>
+      <c r="G7" s="1" t="s">
+        <v>78</v>
+      </c>
       <c r="H7" s="1"/>
     </row>
     <row r="8" spans="1:8">
@@ -1094,7 +1099,9 @@
       <c r="F8" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="G8" s="1"/>
+      <c r="G8" s="1" t="s">
+        <v>69</v>
+      </c>
       <c r="H8" s="1"/>
     </row>
     <row r="9" spans="1:8">
@@ -1136,7 +1143,9 @@
       <c r="F10" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="G10" s="1"/>
+      <c r="G10" s="1" t="s">
+        <v>78</v>
+      </c>
       <c r="H10" s="1"/>
     </row>
     <row r="11" spans="1:8">
@@ -1404,7 +1413,9 @@
         <v>24</v>
       </c>
       <c r="F24" s="5"/>
-      <c r="G24" s="1"/>
+      <c r="G24" s="1" t="s">
+        <v>69</v>
+      </c>
       <c r="H24" s="14"/>
     </row>
     <row r="25" spans="1:8">
@@ -1422,7 +1433,9 @@
         <v>24</v>
       </c>
       <c r="F25" s="5"/>
-      <c r="G25" s="1"/>
+      <c r="G25" s="1" t="s">
+        <v>69</v>
+      </c>
       <c r="H25" s="14"/>
     </row>
     <row r="26" spans="1:8">
@@ -1440,7 +1453,9 @@
         <v>24</v>
       </c>
       <c r="F26" s="5"/>
-      <c r="G26" s="1"/>
+      <c r="G26" s="1" t="s">
+        <v>69</v>
+      </c>
       <c r="H26" s="14"/>
     </row>
     <row r="27" spans="1:8">
@@ -1776,7 +1791,9 @@
       <c r="F42" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="G42" s="1"/>
+      <c r="G42" s="1" t="s">
+        <v>78</v>
+      </c>
       <c r="H42" s="1"/>
     </row>
     <row r="43" spans="1:8" ht="27">

</xml_diff>